<commit_message>
made changes for ecel by adding locatorvalue column
</commit_message>
<xml_diff>
--- a/KeyWordDrivenHubSpot/src/main/java/com/qa/hs/keyword/scenarios/KeyWordHubSpot.xlsx
+++ b/KeyWordDrivenHubSpot/src/main/java/com/qa/hs/keyword/scenarios/KeyWordHubSpot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14050" windowHeight="3320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18460" windowHeight="5570"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>test step</t>
   </si>
   <si>
-    <t>locator</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -64,13 +61,22 @@
     <t>https://classic.crmpro.com/index.html</t>
   </si>
   <si>
-    <t>name = password</t>
-  </si>
-  <si>
-    <t>name = username</t>
-  </si>
-  <si>
     <t>sendKeys</t>
+  </si>
+  <si>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>locatorValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name  </t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -406,96 +412,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.26953125" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="43.26953125" customWidth="1"/>
+    <col min="2" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="43.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:5" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:5" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>